<commit_message>
update to current profile
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.bloodSugarB.xlsx
+++ b/docs/StructureDefinition-VA.MHV.bloodSugarB.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="529">
   <si>
     <t>Path</t>
   </si>
@@ -743,6 +743,9 @@
   </si>
   <si>
     <t>Observation.code.coding</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>4</t>
@@ -4943,7 +4946,7 @@
         <v>231</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>45</v>
@@ -4958,16 +4961,16 @@
         <v>109</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -5004,17 +5007,17 @@
         <v>45</v>
       </c>
       <c r="AA27" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AB27" s="2"/>
       <c r="AC27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD27" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -5035,10 +5038,10 @@
         <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
@@ -5052,7 +5055,7 @@
         <v>230</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C28" t="s" s="2">
         <v>45</v>
@@ -5077,16 +5080,16 @@
         <v>109</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -5096,7 +5099,7 @@
         <v>45</v>
       </c>
       <c r="R28" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="S28" t="s" s="2">
         <v>45</v>
@@ -5135,7 +5138,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -5156,10 +5159,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -5173,7 +5176,7 @@
         <v>230</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C29" t="s" s="2">
         <v>45</v>
@@ -5198,16 +5201,16 @@
         <v>109</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
@@ -5217,7 +5220,7 @@
         <v>45</v>
       </c>
       <c r="R29" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="S29" t="s" s="2">
         <v>45</v>
@@ -5256,7 +5259,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -5277,10 +5280,10 @@
         <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
@@ -5294,14 +5297,14 @@
         <v>230</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>55</v>
@@ -5319,16 +5322,16 @@
         <v>109</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -5338,7 +5341,7 @@
         <v>45</v>
       </c>
       <c r="R30" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="S30" t="s" s="2">
         <v>45</v>
@@ -5377,7 +5380,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5398,10 +5401,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5415,14 +5418,14 @@
         <v>230</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>55</v>
@@ -5440,16 +5443,16 @@
         <v>109</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5459,7 +5462,7 @@
         <v>45</v>
       </c>
       <c r="R31" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="S31" t="s" s="2">
         <v>45</v>
@@ -5498,7 +5501,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5519,10 +5522,10 @@
         <v>45</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5533,7 +5536,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5559,16 +5562,16 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
@@ -5617,7 +5620,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5638,10 +5641,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5652,7 +5655,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5675,19 +5678,19 @@
         <v>56</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5736,7 +5739,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5751,19 +5754,19 @@
         <v>67</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AO33" t="s" s="2">
         <v>45</v>
@@ -5771,7 +5774,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5794,16 +5797,16 @@
         <v>56</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5853,7 +5856,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5877,10 +5880,10 @@
         <v>224</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>45</v>
@@ -5888,11 +5891,11 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -5911,19 +5914,19 @@
         <v>56</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
@@ -5972,7 +5975,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5987,19 +5990,19 @@
         <v>67</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>45</v>
@@ -6007,11 +6010,11 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -6030,19 +6033,19 @@
         <v>56</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -6079,17 +6082,17 @@
         <v>45</v>
       </c>
       <c r="AA36" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AB36" s="2"/>
       <c r="AC36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD36" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -6104,19 +6107,19 @@
         <v>67</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>45</v>
@@ -6124,13 +6127,13 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
@@ -6149,19 +6152,19 @@
         <v>56</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -6210,7 +6213,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -6225,19 +6228,19 @@
         <v>67</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>45</v>
@@ -6245,7 +6248,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6271,13 +6274,13 @@
         <v>91</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -6327,7 +6330,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6348,13 +6351,13 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>45</v>
@@ -6362,7 +6365,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6385,17 +6388,17 @@
         <v>56</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6444,7 +6447,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6459,19 +6462,19 @@
         <v>67</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>45</v>
@@ -6479,7 +6482,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6502,19 +6505,19 @@
         <v>56</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6551,17 +6554,17 @@
         <v>45</v>
       </c>
       <c r="AA40" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AB40" s="2"/>
       <c r="AC40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD40" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6570,7 +6573,7 @@
         <v>55</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>67</v>
@@ -6579,27 +6582,27 @@
         <v>45</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C41" t="s" s="2">
         <v>45</v>
@@ -6621,19 +6624,19 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6682,7 +6685,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6691,7 +6694,7 @@
         <v>55</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>67</v>
@@ -6700,24 +6703,24 @@
         <v>45</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6832,7 +6835,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6949,7 +6952,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6972,19 +6975,19 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -7033,7 +7036,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -7054,10 +7057,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -7068,7 +7071,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -7094,20 +7097,20 @@
         <v>132</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P45" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q45" t="s" s="2">
         <v>45</v>
@@ -7131,10 +7134,10 @@
         <v>195</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="Z45" t="s" s="2">
         <v>45</v>
@@ -7152,7 +7155,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -7173,10 +7176,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -7187,7 +7190,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7213,14 +7216,14 @@
         <v>57</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>45</v>
@@ -7230,7 +7233,7 @@
         <v>45</v>
       </c>
       <c r="R46" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="S46" t="s" s="2">
         <v>45</v>
@@ -7269,7 +7272,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7290,10 +7293,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -7304,7 +7307,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7330,14 +7333,14 @@
         <v>97</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -7386,7 +7389,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7395,7 +7398,7 @@
         <v>55</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>67</v>
@@ -7407,10 +7410,10 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7421,7 +7424,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7447,16 +7450,16 @@
         <v>132</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7505,7 +7508,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7526,10 +7529,10 @@
         <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7540,7 +7543,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7566,16 +7569,16 @@
         <v>204</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7603,10 +7606,10 @@
         <v>113</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7624,7 +7627,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7633,7 +7636,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7648,7 +7651,7 @@
         <v>155</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7659,11 +7662,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7685,16 +7688,16 @@
         <v>204</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7722,10 +7725,10 @@
         <v>113</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7743,7 +7746,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7761,24 +7764,24 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7801,19 +7804,19 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7862,7 +7865,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7883,10 +7886,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7897,7 +7900,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7923,13 +7926,13 @@
         <v>204</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7958,10 +7961,10 @@
         <v>122</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7979,7 +7982,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7997,24 +8000,24 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -8040,16 +8043,16 @@
         <v>204</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -8078,7 +8081,7 @@
       </c>
       <c r="X53" s="2"/>
       <c r="Y53" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -8096,7 +8099,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -8117,10 +8120,10 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -8131,7 +8134,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -8154,16 +8157,16 @@
         <v>45</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
@@ -8213,7 +8216,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8231,24 +8234,24 @@
         <v>45</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8271,16 +8274,16 @@
         <v>45</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -8330,7 +8333,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8348,24 +8351,24 @@
         <v>45</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO55" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8388,19 +8391,19 @@
         <v>45</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8449,7 +8452,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8461,7 +8464,7 @@
         <v>45</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>45</v>
@@ -8470,10 +8473,10 @@
         <v>45</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>45</v>
@@ -8484,7 +8487,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8599,7 +8602,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8716,11 +8719,11 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
@@ -8742,16 +8745,16 @@
         <v>75</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M59" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8800,7 +8803,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8835,7 +8838,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8858,13 +8861,13 @@
         <v>45</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -8915,7 +8918,7 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -8924,7 +8927,7 @@
         <v>55</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI60" t="s" s="2">
         <v>67</v>
@@ -8936,10 +8939,10 @@
         <v>45</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
@@ -8950,7 +8953,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8973,13 +8976,13 @@
         <v>45</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -9030,7 +9033,7 @@
         <v>45</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
@@ -9039,7 +9042,7 @@
         <v>55</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>67</v>
@@ -9051,10 +9054,10 @@
         <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -9065,7 +9068,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -9091,16 +9094,16 @@
         <v>204</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>45</v>
@@ -9128,10 +9131,10 @@
         <v>136</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>45</v>
@@ -9149,7 +9152,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -9167,13 +9170,13 @@
         <v>45</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>45</v>
@@ -9184,7 +9187,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9210,16 +9213,16 @@
         <v>204</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>45</v>
@@ -9247,10 +9250,10 @@
         <v>122</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>45</v>
@@ -9268,7 +9271,7 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -9286,13 +9289,13 @@
         <v>45</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>45</v>
@@ -9303,7 +9306,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9326,17 +9329,17 @@
         <v>45</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>45</v>
@@ -9385,7 +9388,7 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
@@ -9409,7 +9412,7 @@
         <v>45</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
@@ -9420,7 +9423,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9446,10 +9449,10 @@
         <v>57</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -9500,7 +9503,7 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>43</v>
@@ -9521,10 +9524,10 @@
         <v>45</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>45</v>
@@ -9535,7 +9538,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9558,16 +9561,16 @@
         <v>56</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -9617,7 +9620,7 @@
         <v>45</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>43</v>
@@ -9638,10 +9641,10 @@
         <v>45</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>45</v>
@@ -9652,7 +9655,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9675,16 +9678,16 @@
         <v>56</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
@@ -9734,7 +9737,7 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
@@ -9755,10 +9758,10 @@
         <v>45</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>45</v>
@@ -9769,7 +9772,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9792,19 +9795,19 @@
         <v>56</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>45</v>
@@ -9853,7 +9856,7 @@
         <v>45</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>43</v>
@@ -9874,10 +9877,10 @@
         <v>45</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>
@@ -9888,7 +9891,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -10003,7 +10006,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10120,11 +10123,11 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
@@ -10146,16 +10149,16 @@
         <v>75</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M71" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>45</v>
@@ -10204,7 +10207,7 @@
         <v>45</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>43</v>
@@ -10239,7 +10242,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -10265,13 +10268,13 @@
         <v>204</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="N72" t="s" s="2">
         <v>219</v>
@@ -10323,7 +10326,7 @@
         <v>45</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>55</v>
@@ -10341,7 +10344,7 @@
         <v>45</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>224</v>
@@ -10358,7 +10361,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -10381,19 +10384,19 @@
         <v>56</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>45</v>
@@ -10442,7 +10445,7 @@
         <v>45</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>43</v>
@@ -10460,24 +10463,24 @@
         <v>45</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO73" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10503,16 +10506,16 @@
         <v>204</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="O74" t="s" s="2">
         <v>45</v>
@@ -10540,10 +10543,10 @@
         <v>113</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="Z74" t="s" s="2">
         <v>45</v>
@@ -10561,7 +10564,7 @@
         <v>45</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>43</v>
@@ -10570,7 +10573,7 @@
         <v>55</v>
       </c>
       <c r="AH74" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AI74" t="s" s="2">
         <v>67</v>
@@ -10585,7 +10588,7 @@
         <v>155</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>45</v>
@@ -10596,11 +10599,11 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
@@ -10622,16 +10625,16 @@
         <v>204</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N75" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="O75" t="s" s="2">
         <v>45</v>
@@ -10659,10 +10662,10 @@
         <v>113</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="Z75" t="s" s="2">
         <v>45</v>
@@ -10680,7 +10683,7 @@
         <v>45</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>43</v>
@@ -10698,24 +10701,24 @@
         <v>45</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO75" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -10741,16 +10744,16 @@
         <v>45</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N76" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>45</v>
@@ -10799,7 +10802,7 @@
         <v>45</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>43</v>
@@ -10820,10 +10823,10 @@
         <v>45</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>45</v>

</xml_diff>